<commit_message>
Final Sync: PIM stabilization and data-driven logic fully restored
</commit_message>
<xml_diff>
--- a/src/main/resources/data/OrangeHrmData.xlsx
+++ b/src/main/resources/data/OrangeHrmData.xlsx
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+  <si>
+    <t>TestCaseName</t>
+  </si>
   <si>
     <t>username</t>
   </si>
@@ -27,6 +30,9 @@
     <t>expectedMessage</t>
   </si>
   <si>
+    <t>validLogin</t>
+  </si>
+  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -36,10 +42,16 @@
     <t>Success</t>
   </si>
   <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Invalid cedentials</t>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>invalidUsername</t>
   </si>
   <si>
     <t>Admi</t>
@@ -48,16 +60,22 @@
     <t>admin123</t>
   </si>
   <si>
+    <t>invalidUsernameAndPassword</t>
+  </si>
+  <si>
     <t>admin1</t>
   </si>
   <si>
-    <t>Empty Username</t>
-  </si>
-  <si>
-    <t>Empty Password</t>
-  </si>
-  <si>
-    <t>Empty Username and Password</t>
+    <t>emptyUsername</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>emptyPassword</t>
+  </si>
+  <si>
+    <t>emptyUsernameAndPassword</t>
   </si>
   <si>
     <t>firstName</t>
@@ -99,7 +117,7 @@
     <t>Jay</t>
   </si>
   <si>
-    <t>smitjaynedav</t>
+    <t>smitjaytbaser</t>
   </si>
   <si>
     <t>P@ssw0rd123</t>
@@ -156,7 +174,7 @@
     <t>Password123!</t>
   </si>
   <si>
-    <t>0388</t>
+    <t>0407</t>
   </si>
 </sst>
 </file>
@@ -460,13 +478,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="28.75"/>
+    <col min="1" max="1" customWidth="true" width="24.63"/>
+    <col min="4" max="4" customWidth="true" width="28.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,70 +498,94 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6">
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="1" t="s">
-        <v>13</v>
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -569,72 +612,72 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I2" s="5">
         <v>46024.0</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -655,62 +698,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -731,15 +774,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>